<commit_message>
adding room navigation and updating example excel file
</commit_message>
<xml_diff>
--- a/uploads/sample_files/example_excel_format.xlsx
+++ b/uploads/sample_files/example_excel_format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\UofSC School\TheBackyardigans\uploads\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033A434F-6F93-44F0-A5F2-8122ED986A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD122BB-3DEF-4F6E-B51D-A4165E445C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
   <si>
     <t>Descriptor</t>
   </si>
@@ -71,40 +71,52 @@
     <t>WINDOW</t>
   </si>
   <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Sensor LW67756</t>
+  </si>
+  <si>
     <t>rotation</t>
   </si>
   <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Camera A</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>DOOR</t>
+  </si>
+  <si>
+    <t>door_length</t>
+  </si>
+  <si>
     <t>door_angle</t>
   </si>
   <si>
-    <t>door_length</t>
-  </si>
-  <si>
     <t>door_xory</t>
   </si>
   <si>
-    <t>Calibration</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
-  <si>
-    <t>Camera A</t>
-  </si>
-  <si>
-    <t>Sensor</t>
-  </si>
-  <si>
-    <t>Sensor LW67756</t>
-  </si>
-  <si>
-    <t>DOOR</t>
-  </si>
-  <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Room Navigation</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>room_nav_direction</t>
   </si>
 </sst>
 </file>
@@ -456,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECC682-D3AC-405B-A5DD-FF93AD75680E}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -484,24 +496,27 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>72</v>
@@ -510,12 +525,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>72</v>
@@ -527,12 +542,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>72</v>
@@ -541,7 +556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -561,7 +576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -581,7 +596,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -595,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -609,7 +624,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -623,7 +638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -637,7 +652,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -651,7 +666,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -665,7 +680,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -679,7 +694,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -693,7 +708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -707,7 +722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -721,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -735,12 +750,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>75</v>
@@ -758,7 +773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -772,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -784,6 +799,23 @@
       </c>
       <c r="D20">
         <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>125</v>
+      </c>
+      <c r="D21">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing furniture template to updated ASSET style along with example excel sheet
</commit_message>
<xml_diff>
--- a/uploads/sample_files/example_excel_format.xlsx
+++ b/uploads/sample_files/example_excel_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD122BB-3DEF-4F6E-B51D-A4165E445C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A80B9-0E8D-4EF3-9623-71386C6E7D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>Descriptor</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>room_nav_direction</t>
+  </si>
+  <si>
+    <t>furniture_type</t>
+  </si>
+  <si>
+    <t>rectangle</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>radius</t>
   </si>
 </sst>
 </file>
@@ -468,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECC682-D3AC-405B-A5DD-FF93AD75680E}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -510,8 +522,14 @@
       <c r="K1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -525,7 +543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -542,7 +560,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -556,7 +574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -575,8 +593,14 @@
       <c r="F5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -589,14 +613,14 @@
       <c r="D6">
         <v>80</v>
       </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -610,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -624,7 +648,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -638,7 +662,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -652,7 +676,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -666,7 +690,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -680,7 +704,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -694,7 +718,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -708,7 +732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -722,7 +746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
adding basic gridline options and updating example excel
</commit_message>
<xml_diff>
--- a/uploads/sample_files/example_excel_format.xlsx
+++ b/uploads/sample_files/example_excel_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A80B9-0E8D-4EF3-9623-71386C6E7D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E4C90B-4A06-4D7D-92C3-A360671A6476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>Descriptor</t>
   </si>
@@ -129,6 +129,21 @@
   </si>
   <si>
     <t>radius</t>
+  </si>
+  <si>
+    <t>X Axis</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Y Axis</t>
+  </si>
+  <si>
+    <t>step</t>
   </si>
 </sst>
 </file>
@@ -480,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECC682-D3AC-405B-A5DD-FF93AD75680E}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -528,236 +543,245 @@
       <c r="N1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2">
+        <v>-36</v>
+      </c>
+      <c r="P2">
+        <v>144</v>
+      </c>
+      <c r="Q2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>180</v>
+      </c>
+      <c r="Q3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="C2">
-        <v>72</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>72</v>
-      </c>
-      <c r="D3">
-        <v>72</v>
-      </c>
-      <c r="G3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>72</v>
       </c>
       <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="G5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>72</v>
+      </c>
+      <c r="D6">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>26</v>
       </c>
-      <c r="D5">
+      <c r="D7">
         <v>34.5</v>
       </c>
-      <c r="E5">
+      <c r="E7">
         <v>24</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>24</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>80</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M8" t="s">
         <v>29</v>
       </c>
-      <c r="N6">
+      <c r="N8">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>50</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>50</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-      <c r="D12">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>100</v>
       </c>
       <c r="D13">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
       <c r="D14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>100</v>
       </c>
       <c r="D15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -768,10 +792,10 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -779,22 +803,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <v>0</v>
-      </c>
-      <c r="H18">
-        <v>10</v>
-      </c>
-      <c r="I18">
-        <v>-50</v>
-      </c>
-      <c r="J18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -805,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -816,29 +831,66 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D20">
         <v>0</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>-50</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>125</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>25</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K23" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating all sample files
</commit_message>
<xml_diff>
--- a/uploads/sample_files/example_excel_format.xlsx
+++ b/uploads/sample_files/example_excel_format.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\UofSC School\TheBackyardigans\uploads\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F8C3C3-24F4-4BB2-92C1-7A8DAB0F0D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C5271E-3C6C-4091-AC3B-FA8B0068EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECC682-D3AC-405B-A5DD-FF93AD75680E}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,7 +537,7 @@
     <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -571,23 +571,23 @@
       <c r="K1" t="s">
         <v>26</v>
       </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -595,7 +595,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -603,7 +603,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -611,7 +611,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -619,7 +619,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -627,35 +627,35 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
+      <c r="N7">
+        <v>-36</v>
+      </c>
       <c r="O7">
-        <v>-36</v>
+        <v>288</v>
       </c>
       <c r="P7">
-        <v>288</v>
-      </c>
-      <c r="Q7">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
       <c r="O8">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="P8">
-        <v>180</v>
-      </c>
-      <c r="Q8">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -669,7 +669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -686,7 +686,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -700,7 +700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -722,11 +722,11 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="M12" t="s">
+      <c r="L12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -739,14 +739,14 @@
       <c r="D13">
         <v>80</v>
       </c>
-      <c r="M13" t="s">
+      <c r="L13" t="s">
         <v>29</v>
       </c>
-      <c r="N13">
+      <c r="M13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -760,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -774,7 +774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -970,5 +970,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>